<commit_message>
Minor formatting For future reference, minor formatting just means adjusting column width to fit.
</commit_message>
<xml_diff>
--- a/Excel Workbooks/100/100Pi1.xlsx
+++ b/Excel Workbooks/100/100Pi1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\StatsProject\Excel Workbooks\100\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B810418C-D799-4E5F-BCFB-CB7191CC6549}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -40,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +84,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -124,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -156,9 +170,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,6 +222,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -365,14 +415,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,12 +441,12 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.522462374304468</v>
+        <v>0.52246237430446796</v>
       </c>
       <c r="B2">
-        <v>0.08387718904855634</v>
+        <v>8.3877189048556344E-2</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -400,26 +455,26 @@
         <v>0.1784073464102067</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.3291548324339415</v>
       </c>
       <c r="B3">
-        <v>0.100623862453019</v>
+        <v>0.10062386245301901</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3">
-        <v>5.678882213018502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>5.6788822130185022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.6086631515149429</v>
+        <v>0.60866315151494288</v>
       </c>
       <c r="B4">
-        <v>0.2186372249696983</v>
+        <v>0.21863722496969831</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -428,423 +483,423 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.9264625624142935</v>
+        <v>0.92646256241429348</v>
       </c>
       <c r="B5">
-        <v>0.7308740277582363</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.73087402775823629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.03572309869638324</v>
+        <v>3.5723098696383238E-2</v>
       </c>
       <c r="B6">
-        <v>0.9812862265135806</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0.98128622651358055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.9351764792635087</v>
+        <v>0.93517647926350866</v>
       </c>
       <c r="B7">
-        <v>0.2639202643325682</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>0.26392026433256821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.09642803125970367</v>
+        <v>9.6428031259703673E-2</v>
       </c>
       <c r="B8">
         <v>0.1180066246906032</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.659420710196478</v>
+        <v>0.65942071019647797</v>
       </c>
       <c r="B9">
-        <v>0.5960517808903376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>0.59605178089033761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.442981253640447</v>
+        <v>0.44298125364044699</v>
       </c>
       <c r="B10">
-        <v>0.4818576182100722</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>0.48185761821007222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.1997646005263781</v>
+        <v>0.19976460052637809</v>
       </c>
       <c r="B11">
-        <v>0.2669849470951173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>0.26698494709511728</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.3908697827549714</v>
+        <v>0.39086978275497142</v>
       </c>
       <c r="B12">
         <v>0.5815639999869856</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.7090496772966758</v>
+        <v>0.70904967729667578</v>
       </c>
       <c r="B13">
         <v>0.2009789828606289</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.4604417213213855</v>
       </c>
       <c r="B14">
-        <v>0.3152445537805749</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>0.31524455378057492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.265347702613438</v>
+        <v>0.26534770261343799</v>
       </c>
       <c r="B15">
-        <v>0.2461798035546721</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>0.24617980355467209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.2567133373771771</v>
+        <v>0.25671333737717711</v>
       </c>
       <c r="B16">
-        <v>0.2000737774986079</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>0.20007377749860791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.6058052445979351</v>
+        <v>0.60580524459793506</v>
       </c>
       <c r="B17">
-        <v>0.001671697954224727</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>1.671697954224727E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.5608019965675008</v>
+        <v>0.56080199656750085</v>
       </c>
       <c r="B18">
-        <v>0.3023037119706615</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>0.30230371197066153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.7344162320999744</v>
+        <v>0.73441623209997442</v>
       </c>
       <c r="B19">
-        <v>0.4905033318377571</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>0.49050333183775707</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.8188784778361733</v>
+        <v>0.81887847783617329</v>
       </c>
       <c r="B20">
-        <v>0.05241374231905849</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>5.2413742319058487E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.7744679422238491</v>
+        <v>0.77446794222384907</v>
       </c>
       <c r="B21">
-        <v>0.6802553912400653</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>0.68025539124006529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.632157309827048</v>
+        <v>0.63215730982704799</v>
       </c>
       <c r="B22">
-        <v>0.2144821433437769</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>0.21448214334377691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.9727445369656788</v>
+        <v>0.97274453696567875</v>
       </c>
       <c r="B23">
-        <v>0.471020169239443</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>0.47102016923944301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.09957066366231559</v>
+        <v>9.9570663662315595E-2</v>
       </c>
       <c r="B24">
-        <v>0.8463905856048655</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>0.84639058560486546</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.1171577478103882</v>
+        <v>0.11715774781038819</v>
       </c>
       <c r="B25">
-        <v>0.09405794440711635</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>9.4057944407116345E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.7839918189012068</v>
+        <v>0.78399181890120684</v>
       </c>
       <c r="B26">
-        <v>0.8757206709694307</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>0.87572067096943074</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.1845783823140951</v>
       </c>
       <c r="B27">
-        <v>0.3997833997396508</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>0.39978339973965082</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.8714460962533022</v>
+        <v>0.87144609625330216</v>
       </c>
       <c r="B28">
         <v>0.2296870311605865</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.2421132527692661</v>
       </c>
       <c r="B29">
-        <v>0.4946018721464122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>0.49460187214641221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.3401311253568269</v>
+        <v>0.34013112535682688</v>
       </c>
       <c r="B30">
-        <v>0.9151899373095285</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>0.91518993730952847</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.946009665208803</v>
+        <v>0.94600966520880303</v>
       </c>
       <c r="B31">
-        <v>0.04652234184507964</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>4.652234184507964E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.4369709114964263</v>
+        <v>0.43697091149642631</v>
       </c>
       <c r="B32">
-        <v>0.7974615402296379</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>0.79746154022963789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.5892229004427516</v>
+        <v>0.58922290044275161</v>
       </c>
       <c r="B33">
-        <v>0.5734436630918665</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>0.57344366309186645</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.1222972780029002</v>
       </c>
       <c r="B34">
-        <v>0.66854780024738</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>0.66854780024738003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.7098478457529847</v>
+        <v>0.70984784575298465</v>
       </c>
       <c r="B35">
-        <v>0.9822071348523853</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>0.98220713485238531</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.4535620943356243</v>
+        <v>0.45356209433562428</v>
       </c>
       <c r="B36">
-        <v>0.1689234092844299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>0.16892340928442989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0.8897497153259241</v>
+        <v>0.88974971532592406</v>
       </c>
       <c r="B37">
-        <v>0.7704682310313717</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>0.77046823103137174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.7494339420526284</v>
+        <v>0.74943394205262837</v>
       </c>
       <c r="B38">
-        <v>0.3100878065772164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>0.31008780657721641</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0.6158597603865084</v>
+        <v>0.61585976038650836</v>
       </c>
       <c r="B39">
-        <v>0.2277569945617973</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>0.22775699456179729</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0.794700888784885</v>
+        <v>0.79470088878488498</v>
       </c>
       <c r="B40">
-        <v>0.003202440170699927</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>3.2024401706999268E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0.2999260403771075</v>
+        <v>0.29992604037710752</v>
       </c>
       <c r="B41">
-        <v>0.7316460488227848</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>0.73164604882278483</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0.3799925869153118</v>
+        <v>0.37999258691531179</v>
       </c>
       <c r="B42">
-        <v>0.3434202084957337</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>0.34342020849573368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>0.4493062050102029</v>
+        <v>0.44930620501020291</v>
       </c>
       <c r="B43">
-        <v>0.5192519875908252</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>0.51925198759082525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0.6964573750400977</v>
+        <v>0.69645737504009775</v>
       </c>
       <c r="B44">
-        <v>0.7379020344457963</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>0.73790203444579627</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0.1352421674077118</v>
+        <v>0.13524216740771181</v>
       </c>
       <c r="B45">
-        <v>0.7634324917453003</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>0.76343249174530026</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0.5015359713991906</v>
+        <v>0.50153597139919059</v>
       </c>
       <c r="B46">
-        <v>0.765165371747383</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>0.76516537174738297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.5406072686473361</v>
       </c>
       <c r="B47">
-        <v>0.04772133472391904</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>4.772133472391904E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>0.4938742230639698</v>
+        <v>0.49387422306396978</v>
       </c>
       <c r="B48">
-        <v>0.9877144765379831</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>0.98771447653798305</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.9657148667294948</v>
       </c>
       <c r="B49">
-        <v>0.7529425664180032</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>0.75294256641800317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>0.381732933977363</v>
+        <v>0.38173293397736302</v>
       </c>
       <c r="B50">
-        <v>0.590546444429223</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>0.59054644442922299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>0.6530489773522531</v>
+        <v>0.65304897735225309</v>
       </c>
       <c r="B51">
-        <v>0.6081378521037564</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>0.60813785210375637</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>0.5604686412858307</v>
+        <v>0.56046864128583074</v>
       </c>
       <c r="B52">
         <v>0.6547761509431077</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>0.4204525102394037</v>
+        <v>0.42045251023940372</v>
       </c>
       <c r="B53">
-        <v>0.2882859923293641</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>0.28828599232936408</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0.7373599638822634</v>
+        <v>0.73735996388226344</v>
       </c>
       <c r="B54">
-        <v>0.5118360691623324</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>0.51183606916233237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>0.03942643210306895</v>
+        <v>3.9426432103068947E-2</v>
       </c>
       <c r="B55">
-        <v>0.7315424853523516</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>0.73154248535235156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>0.1419230372707253</v>
+        <v>0.14192303727072531</v>
       </c>
       <c r="B56">
-        <v>0.818650709009854</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>0.81865070900985404</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.9021916620618804</v>
       </c>
@@ -852,55 +907,55 @@
         <v>0.5597078626222709</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0.152338081666503</v>
+        <v>0.15233808166650301</v>
       </c>
       <c r="B58">
-        <v>0.9132224461936453</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>0.91322244619364534</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0.9121345376101286</v>
+        <v>0.91213453761012864</v>
       </c>
       <c r="B59">
-        <v>0.3047736308490567</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>0.30477363084905668</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>0.4171495757654538</v>
+        <v>0.41714957576545381</v>
       </c>
       <c r="B60">
-        <v>0.6745201799973863</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>0.67452017999738634</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.362020607320646</v>
       </c>
       <c r="B61">
-        <v>0.02575203569731777</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>2.5752035697317769E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.5174870225047149</v>
       </c>
       <c r="B62">
-        <v>0.8211590354609221</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>0.82115903546092206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>0.8979349858994816</v>
+        <v>0.89793498589948162</v>
       </c>
       <c r="B63">
         <v>0.1427410119858997</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.2262591145768984</v>
       </c>
@@ -908,300 +963,300 @@
         <v>0.8698609345058852</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0.6488048675778507</v>
+        <v>0.64880486757785072</v>
       </c>
       <c r="B65">
-        <v>0.675534996303556</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>0.67553499630355596</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>0.5877083948397794</v>
+        <v>0.58770839483977944</v>
       </c>
       <c r="B66">
-        <v>0.7495461974050778</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>0.74954619740507777</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0.3367554013233975</v>
+        <v>0.33675540132339749</v>
       </c>
       <c r="B67">
-        <v>0.5653749912793977</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>0.56537499127939772</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>0.8754877120254767</v>
+        <v>0.87548771202547671</v>
       </c>
       <c r="B68">
         <v>0.7178426319454122</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.1754400753886389</v>
       </c>
       <c r="B69">
-        <v>0.03904766138610516</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>3.9047661386105159E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>0.6109383609585429</v>
+        <v>0.61093836095854293</v>
       </c>
       <c r="B70">
-        <v>0.3867419728585414</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>0.38674197285854139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.4444210710739217</v>
       </c>
       <c r="B71">
-        <v>0.6315104087074304</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>0.63151040870743036</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.9794876723099476</v>
       </c>
       <c r="B72">
-        <v>0.6480508938624555</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>0.64805089386245551</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.5018005509158705</v>
       </c>
       <c r="B73">
-        <v>0.4029276369803705</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>0.40292763698037048</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>0.3641465776293851</v>
+        <v>0.36414657762938513</v>
       </c>
       <c r="B74">
-        <v>0.4692249346042842</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>0.46922493460428422</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>0.8735512737032387</v>
+        <v>0.87355127370323871</v>
       </c>
       <c r="B75">
-        <v>0.91704193689688</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>0.91704193689687996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>0.7204947719122778</v>
+        <v>0.72049477191227784</v>
       </c>
       <c r="B76">
-        <v>0.6268780670187218</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>0.62687806701872184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>0.8814868008341668</v>
+        <v>0.88148680083416675</v>
       </c>
       <c r="B77">
-        <v>0.931742095410289</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>0.93174209541028896</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>0.6974240581729519</v>
+        <v>0.69742405817295194</v>
       </c>
       <c r="B78">
-        <v>0.760437145175974</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>0.76043714517597405</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>0.07142852782568299</v>
+        <v>7.1428527825682986E-2</v>
       </c>
       <c r="B79">
-        <v>0.01296942409141089</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>1.296942409141089E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>0.2691702451189205</v>
+        <v>0.26917024511892051</v>
       </c>
       <c r="B80">
-        <v>0.4166318163328409</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>0.41663181633284091</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>0.3069793802807171</v>
+        <v>0.30697938028071708</v>
       </c>
       <c r="B81">
-        <v>0.7871306089819042</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>0.78713060898190423</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>0.841079921449944</v>
+        <v>0.84107992144994403</v>
       </c>
       <c r="B82">
-        <v>0.5609471269802648</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>0.56094712698026483</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>0.2138036030030163</v>
+        <v>0.21380360300301629</v>
       </c>
       <c r="B83">
-        <v>0.3918894506911735</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>0.39188945069117348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0.01294839877544851</v>
+        <v>1.2948398775448511E-2</v>
       </c>
       <c r="B84">
-        <v>0.2848958881767977</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>0.28489588817679767</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.2461966094029969</v>
       </c>
       <c r="B85">
-        <v>0.4123775975382806</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>0.41237759753828063</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.1705423762389405</v>
       </c>
       <c r="B86">
-        <v>0.6279950737517203</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>0.62799507375172026</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.1998913707460892</v>
       </c>
       <c r="B87">
-        <v>0.4463234248008806</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>0.44632342480088061</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0.1609786018779434</v>
+        <v>0.16097860187794341</v>
       </c>
       <c r="B88">
-        <v>0.5177957460653076</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+        <v>0.51779574606530765</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>0.9903077296066343</v>
+        <v>0.99030772960663427</v>
       </c>
       <c r="B89">
-        <v>0.2720329507520856</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>0.27203295075208561</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0.7981307684578768</v>
+        <v>0.79813076845787678</v>
       </c>
       <c r="B90">
-        <v>0.5984843798606512</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>0.59848437986065117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>0.3787573230115676</v>
+        <v>0.37875732301156761</v>
       </c>
       <c r="B91">
-        <v>0.3602514660385504</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>0.36025146603855041</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>0.1662754607072202</v>
+        <v>0.16627546070722021</v>
       </c>
       <c r="B92">
-        <v>0.0688773310586599</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+        <v>6.8877331058659896E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>0.5178598964823879</v>
+        <v>0.51785989648238795</v>
       </c>
       <c r="B93">
-        <v>0.2336209304377637</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>0.23362093043776369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>0.03642630407599767</v>
+        <v>3.6426304075997673E-2</v>
       </c>
       <c r="B94">
-        <v>0.05528847973500661</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>5.5288479735006613E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>0.4254348556832819</v>
+        <v>0.42543485568328188</v>
       </c>
       <c r="B95">
-        <v>0.3757495970940328</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>0.37574959709403277</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>0.2287203610773754</v>
+        <v>0.22872036107737539</v>
       </c>
       <c r="B96">
-        <v>0.001160217999474855</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>1.1602179994748549E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>0.1277096192005797</v>
+        <v>0.12770961920057969</v>
       </c>
       <c r="B97">
-        <v>0.6963049059682019</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>0.69630490596820194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>0.3329605396677022</v>
+        <v>0.33296053966770223</v>
       </c>
       <c r="B98">
-        <v>0.5137245427175883</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>0.51372454271758827</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>0.08882957591389185</v>
+        <v>8.8829575913891845E-2</v>
       </c>
       <c r="B99">
-        <v>0.9329766189457359</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>0.93297661894573591</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>0.01838913211643611</v>
+        <v>1.838913211643611E-2</v>
       </c>
       <c r="B100">
-        <v>0.354126142408442</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>0.35412614240844198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>0.7352618352521481</v>
+        <v>0.73526183525214805</v>
       </c>
       <c r="B101">
-        <v>0.2284921481178888</v>
+        <v>0.22849214811788879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>